<commit_message>
tableau IDF 3e serie
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Travail\Personnel\Squash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Travail\Personnel\Squash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277A77CA-2283-43B6-966E-31A0640671D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4CDBD0-B8AF-4D01-A560-5DFED71347FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
   <si>
     <t>Points</t>
   </si>
@@ -644,7 +644,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,15 +709,15 @@
       </c>
       <c r="G2" s="8">
         <f>SUM(E:E)</f>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H2" s="8">
         <f>SUM(F:F)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I2" s="8">
         <f>SUM(G2:H2)</f>
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -737,11 +737,11 @@
       <c r="F3" s="8"/>
       <c r="G3" s="11">
         <f>G2/I2</f>
-        <v>0.69620253164556967</v>
+        <v>0.68674698795180722</v>
       </c>
       <c r="H3" s="11">
         <f>H2/I2</f>
-        <v>0.30379746835443039</v>
+        <v>0.31325301204819278</v>
       </c>
       <c r="I3" s="8"/>
     </row>
@@ -2023,8 +2023,18 @@
       <c r="I66" s="16"/>
     </row>
     <row r="67" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="16"/>
-      <c r="B67" s="17"/>
+      <c r="A67" s="16">
+        <v>677</v>
+      </c>
+      <c r="B67" s="17">
+        <v>45640</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="E67" s="16"/>
       <c r="F67" s="16"/>
       <c r="G67" s="15"/>
@@ -2032,17 +2042,41 @@
       <c r="I67" s="16"/>
     </row>
     <row r="68" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="16"/>
-      <c r="B68" s="17"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
+      <c r="A68" s="16">
+        <v>907</v>
+      </c>
+      <c r="B68" s="17">
+        <v>45640</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="16">
+        <v>2</v>
+      </c>
+      <c r="F68" s="16">
+        <v>2</v>
+      </c>
       <c r="G68" s="15"/>
       <c r="H68" s="15"/>
       <c r="I68" s="16"/>
     </row>
     <row r="69" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="16"/>
-      <c r="B69" s="17"/>
+      <c r="A69" s="16">
+        <v>907</v>
+      </c>
+      <c r="B69" s="17">
+        <v>45640</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="E69" s="16"/>
       <c r="F69" s="16"/>
       <c r="G69" s="15"/>

</xml_diff>

<commit_message>
Ajout actions IDF 3e série
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Travail\Personnel\Squash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zarka/Documents/Simon/Squash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4CDBD0-B8AF-4D01-A560-5DFED71347FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790EA30D-B462-BE4B-8895-66216923CBBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="1760" windowWidth="32620" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions Simon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="40">
   <si>
     <t>Points</t>
   </si>
@@ -137,16 +124,22 @@
     <t>Paris 19 Place</t>
   </si>
   <si>
-    <t xml:space="preserve">Meudon </t>
+    <t>UCPA Meudon</t>
+  </si>
+  <si>
+    <t>UCPA Meudon Place</t>
+  </si>
+  <si>
+    <t>Savigny</t>
   </si>
   <si>
     <t>Savigny Place</t>
   </si>
   <si>
-    <t>Savigny</t>
-  </si>
-  <si>
-    <t>Blois place</t>
+    <t>3ème Série IdF</t>
+  </si>
+  <si>
+    <t>3ème Série IdF Place</t>
   </si>
 </sst>
 </file>
@@ -156,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +180,16 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri (Corps)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -334,6 +337,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -641,25 +665,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -688,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1">
       <c r="A2" s="8">
         <v>6277</v>
       </c>
@@ -709,18 +733,18 @@
       </c>
       <c r="G2" s="8">
         <f>SUM(E:E)</f>
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H2" s="8">
         <f>SUM(F:F)</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" s="8">
         <f>SUM(G2:H2)</f>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="20.25" customHeight="1">
       <c r="A3" s="8">
         <v>7104</v>
       </c>
@@ -737,15 +761,15 @@
       <c r="F3" s="8"/>
       <c r="G3" s="11">
         <f>G2/I2</f>
-        <v>0.68674698795180722</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="H3" s="11">
         <f>H2/I2</f>
-        <v>0.31325301204819278</v>
+        <v>0.3258426966292135</v>
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1">
       <c r="A4" s="8">
         <v>6332</v>
       </c>
@@ -764,7 +788,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1">
       <c r="A5" s="8">
         <v>5971</v>
       </c>
@@ -787,7 +811,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="19.5" customHeight="1">
       <c r="A6" s="8">
         <v>7104</v>
       </c>
@@ -806,7 +830,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="19.5" customHeight="1">
       <c r="A7" s="8">
         <v>6483</v>
       </c>
@@ -825,7 +849,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="19.5" customHeight="1">
       <c r="A8" s="8">
         <v>4919</v>
       </c>
@@ -848,7 +872,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
     </row>
-    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="19.5" customHeight="1">
       <c r="A9" s="8">
         <v>7191</v>
       </c>
@@ -867,7 +891,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.5" customHeight="1">
       <c r="A10" s="8">
         <v>5564</v>
       </c>
@@ -890,7 +914,7 @@
       <c r="H10" s="15"/>
       <c r="I10" s="16"/>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1">
       <c r="A11" s="8">
         <v>7191</v>
       </c>
@@ -909,7 +933,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1">
       <c r="A12" s="8">
         <v>7191</v>
       </c>
@@ -928,7 +952,7 @@
       <c r="H12" s="15"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1">
       <c r="A13" s="8">
         <v>5564</v>
       </c>
@@ -947,7 +971,7 @@
       <c r="H13" s="15"/>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="19.5" customHeight="1">
       <c r="A14" s="8">
         <v>6639</v>
       </c>
@@ -970,7 +994,7 @@
       <c r="H14" s="15"/>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="19.5" customHeight="1">
       <c r="A15" s="8">
         <v>7191</v>
       </c>
@@ -989,7 +1013,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="19.5" customHeight="1">
       <c r="A16" s="8">
         <v>7155</v>
       </c>
@@ -1008,7 +1032,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="19.5" customHeight="1">
       <c r="A17" s="8">
         <v>4213</v>
       </c>
@@ -1027,7 +1051,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="19.5" customHeight="1">
       <c r="A18" s="8">
         <v>1802</v>
       </c>
@@ -1050,7 +1074,7 @@
       <c r="H18" s="15"/>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1">
       <c r="A19" s="8">
         <v>3347</v>
       </c>
@@ -1073,7 +1097,7 @@
       <c r="H19" s="15"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="19.5" customHeight="1">
       <c r="A20" s="8">
         <v>2298</v>
       </c>
@@ -1092,7 +1116,7 @@
       <c r="H20" s="15"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="19.5" customHeight="1">
       <c r="A21" s="8">
         <v>3293</v>
       </c>
@@ -1111,7 +1135,7 @@
       <c r="H21" s="15"/>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="19.5" customHeight="1">
       <c r="A22" s="8">
         <v>2082</v>
       </c>
@@ -1130,7 +1154,7 @@
       <c r="H22" s="15"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="19.5" customHeight="1">
       <c r="A23" s="8">
         <v>5063</v>
       </c>
@@ -1149,7 +1173,7 @@
       <c r="H23" s="15"/>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="19.5" customHeight="1">
       <c r="A24" s="8">
         <v>2910</v>
       </c>
@@ -1172,7 +1196,7 @@
       <c r="H24" s="15"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="19" customHeight="1">
       <c r="A25" s="8">
         <v>2484</v>
       </c>
@@ -1191,7 +1215,7 @@
       <c r="H25" s="15"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="19" customHeight="1">
       <c r="A26" s="8">
         <v>3071</v>
       </c>
@@ -1210,7 +1234,7 @@
       <c r="H26" s="15"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="19" customHeight="1">
       <c r="A27" s="8">
         <v>2687</v>
       </c>
@@ -1229,7 +1253,7 @@
       <c r="H27" s="15"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="19" customHeight="1">
       <c r="A28" s="8">
         <v>2709</v>
       </c>
@@ -1252,7 +1276,7 @@
       <c r="H28" s="15"/>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="19" customHeight="1">
       <c r="A29" s="8">
         <v>3457</v>
       </c>
@@ -1271,7 +1295,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="19" customHeight="1">
       <c r="A30" s="8">
         <v>4288</v>
       </c>
@@ -1290,7 +1314,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="19" customHeight="1">
       <c r="A31" s="8">
         <v>3457</v>
       </c>
@@ -1309,7 +1333,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="19" customHeight="1">
       <c r="A32" s="8">
         <v>3480</v>
       </c>
@@ -1332,7 +1356,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="19" customHeight="1">
       <c r="A33" s="8">
         <v>2169</v>
       </c>
@@ -1351,7 +1375,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="16"/>
     </row>
-    <row r="34" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="19" customHeight="1">
       <c r="A34" s="8">
         <v>2184</v>
       </c>
@@ -1370,7 +1394,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="16"/>
     </row>
-    <row r="35" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="19.5" customHeight="1">
       <c r="A35" s="8">
         <v>4288</v>
       </c>
@@ -1393,7 +1417,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="16"/>
     </row>
-    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="19.5" customHeight="1">
       <c r="A36" s="8">
         <v>3763</v>
       </c>
@@ -1412,7 +1436,7 @@
       <c r="H36" s="15"/>
       <c r="I36" s="16"/>
     </row>
-    <row r="37" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="19.5" customHeight="1">
       <c r="A37" s="8">
         <v>4288</v>
       </c>
@@ -1431,7 +1455,7 @@
       <c r="H37" s="15"/>
       <c r="I37" s="16"/>
     </row>
-    <row r="38" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="19.5" customHeight="1">
       <c r="A38" s="8">
         <v>2015</v>
       </c>
@@ -1454,7 +1478,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="16"/>
     </row>
-    <row r="39" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="19.5" customHeight="1">
       <c r="A39" s="8">
         <v>1814</v>
       </c>
@@ -1473,7 +1497,7 @@
       <c r="H39" s="15"/>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="19.5" customHeight="1">
       <c r="A40" s="8">
         <v>1829</v>
       </c>
@@ -1492,7 +1516,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="16"/>
     </row>
-    <row r="41" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="19.5" customHeight="1">
       <c r="A41" s="8">
         <v>1387</v>
       </c>
@@ -1515,7 +1539,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="16"/>
     </row>
-    <row r="42" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="19.5" customHeight="1">
       <c r="A42" s="8">
         <v>1321</v>
       </c>
@@ -1534,7 +1558,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="19.5" customHeight="1">
       <c r="A43" s="8">
         <v>1772</v>
       </c>
@@ -1553,7 +1577,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="16"/>
     </row>
-    <row r="44" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="20.25" customHeight="1">
       <c r="A44" s="12">
         <v>1280</v>
       </c>
@@ -1572,7 +1596,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="16"/>
     </row>
-    <row r="45" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="20.25" customHeight="1">
       <c r="A45" s="1">
         <v>2081</v>
       </c>
@@ -1595,7 +1619,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="20.25" customHeight="1">
       <c r="A46" s="1">
         <v>2049</v>
       </c>
@@ -1614,7 +1638,7 @@
       <c r="H46" s="15"/>
       <c r="I46" s="16"/>
     </row>
-    <row r="47" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="19.5" customHeight="1">
       <c r="A47" s="1">
         <v>2081</v>
       </c>
@@ -1637,7 +1661,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="16"/>
     </row>
-    <row r="48" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="19.5" customHeight="1">
       <c r="A48" s="1">
         <v>1296</v>
       </c>
@@ -1660,7 +1684,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="19.5" customHeight="1">
       <c r="A49" s="1">
         <v>2049</v>
       </c>
@@ -1679,7 +1703,7 @@
       <c r="H49" s="15"/>
       <c r="I49" s="16"/>
     </row>
-    <row r="50" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="19.5" customHeight="1">
       <c r="A50" s="1">
         <v>1676</v>
       </c>
@@ -1698,7 +1722,7 @@
       <c r="H50" s="15"/>
       <c r="I50" s="16"/>
     </row>
-    <row r="51" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="19.5" customHeight="1">
       <c r="A51" s="22">
         <v>2081</v>
       </c>
@@ -1721,7 +1745,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="16"/>
     </row>
-    <row r="52" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="19.5" customHeight="1">
       <c r="A52" s="22">
         <v>1970</v>
       </c>
@@ -1740,7 +1764,7 @@
       <c r="H52" s="15"/>
       <c r="I52" s="16"/>
     </row>
-    <row r="53" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="19.5" customHeight="1">
       <c r="A53" s="22">
         <v>476</v>
       </c>
@@ -1763,7 +1787,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="19.5" customHeight="1">
       <c r="A54" s="22">
         <v>1501</v>
       </c>
@@ -1782,7 +1806,7 @@
       <c r="H54" s="15"/>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="19" customHeight="1">
       <c r="A55" s="22">
         <v>476</v>
       </c>
@@ -1801,325 +1825,369 @@
       <c r="H55" s="15"/>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16">
+    <row r="56" spans="1:9" ht="19" customHeight="1">
+      <c r="A56" s="1">
         <v>451</v>
       </c>
-      <c r="B56" s="17">
+      <c r="B56" s="2">
         <v>45612</v>
       </c>
-      <c r="C56" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="16">
+      <c r="C56" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="1">
         <v>3</v>
       </c>
-      <c r="F56" s="16">
+      <c r="F56" s="1">
         <v>1</v>
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
       <c r="I56" s="16"/>
     </row>
-    <row r="57" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16">
+    <row r="57" spans="1:9" ht="19" customHeight="1">
+      <c r="A57" s="1">
         <v>682</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="2">
         <v>45612</v>
       </c>
-      <c r="C57" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="18" t="s">
+      <c r="C57" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
       <c r="I57" s="16"/>
     </row>
-    <row r="58" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="16">
+    <row r="58" spans="1:9" ht="19" customHeight="1">
+      <c r="A58" s="1">
         <v>535</v>
       </c>
-      <c r="B58" s="17">
+      <c r="B58" s="2">
         <v>45612</v>
       </c>
-      <c r="C58" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
+      <c r="C58" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
       <c r="I58" s="16"/>
     </row>
-    <row r="59" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="16">
+    <row r="59" spans="1:9" ht="19" customHeight="1">
+      <c r="A59" s="1">
         <v>641</v>
       </c>
-      <c r="B59" s="17">
+      <c r="B59" s="2">
         <v>45612</v>
       </c>
-      <c r="C59" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
+      <c r="C59" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="16"/>
     </row>
-    <row r="60" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="16">
-        <v>641</v>
-      </c>
-      <c r="B60" s="17">
-        <v>45619</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E60" s="16">
+    <row r="60" spans="1:9" ht="19" customHeight="1">
+      <c r="A60" s="27">
+        <v>1171</v>
+      </c>
+      <c r="B60" s="28">
+        <v>45618</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="27">
         <v>5</v>
       </c>
-      <c r="F60" s="16">
+      <c r="F60" s="27">
         <v>0</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
       <c r="I60" s="16"/>
     </row>
-    <row r="61" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16">
-        <v>641</v>
-      </c>
-      <c r="B61" s="17">
-        <v>45619</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" s="18" t="s">
+    <row r="61" spans="1:9" ht="19" customHeight="1">
+      <c r="A61" s="27">
+        <v>1197</v>
+      </c>
+      <c r="B61" s="28">
+        <v>45618</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
       <c r="I61" s="16"/>
     </row>
-    <row r="62" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="16">
-        <v>1197</v>
-      </c>
-      <c r="B62" s="17">
-        <v>45619</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="18" t="s">
+    <row r="62" spans="1:9" ht="19" customHeight="1">
+      <c r="A62" s="27">
+        <v>641</v>
+      </c>
+      <c r="B62" s="28">
+        <v>45618</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
       <c r="G62" s="15"/>
       <c r="H62" s="15"/>
       <c r="I62" s="16"/>
     </row>
-    <row r="63" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="16">
-        <v>1171</v>
-      </c>
-      <c r="B63" s="17">
-        <v>45619</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
+    <row r="63" spans="1:9" ht="19" customHeight="1">
+      <c r="A63" s="27">
+        <v>641</v>
+      </c>
+      <c r="B63" s="28">
+        <v>45618</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
       <c r="G63" s="15"/>
       <c r="H63" s="15"/>
       <c r="I63" s="16"/>
     </row>
-    <row r="64" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="16">
-        <v>1111</v>
-      </c>
-      <c r="B64" s="17">
+    <row r="64" spans="1:9" ht="19" customHeight="1">
+      <c r="A64" s="1">
+        <v>1069</v>
+      </c>
+      <c r="B64" s="2">
         <v>45626</v>
       </c>
-      <c r="C64" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E64" s="16">
+      <c r="C64" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="1">
         <v>2</v>
       </c>
-      <c r="F64" s="16">
+      <c r="F64" s="1">
         <v>1</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="15"/>
       <c r="I64" s="16"/>
     </row>
-    <row r="65" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16">
+    <row r="65" spans="1:9" ht="19" customHeight="1">
+      <c r="A65" s="1">
         <v>1153</v>
       </c>
-      <c r="B65" s="17">
+      <c r="B65" s="2">
         <v>45626</v>
       </c>
-      <c r="C65" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65" s="18" t="s">
+      <c r="C65" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
       <c r="I65" s="16"/>
     </row>
-    <row r="66" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16">
-        <v>1069</v>
-      </c>
-      <c r="B66" s="17">
+    <row r="66" spans="1:9" ht="19" customHeight="1">
+      <c r="A66" s="1">
+        <v>1111</v>
+      </c>
+      <c r="B66" s="2">
         <v>45626</v>
       </c>
-      <c r="C66" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
+      <c r="C66" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
       <c r="G66" s="15"/>
       <c r="H66" s="15"/>
       <c r="I66" s="16"/>
     </row>
-    <row r="67" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="16">
-        <v>677</v>
-      </c>
-      <c r="B67" s="17">
-        <v>45640</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" s="18" t="s">
+    <row r="67" spans="1:9" ht="19" customHeight="1">
+      <c r="A67" s="1">
+        <v>907</v>
+      </c>
+      <c r="B67" s="2">
+        <v>45639</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="E67" s="1">
+        <v>2</v>
+      </c>
+      <c r="F67" s="1">
+        <v>2</v>
+      </c>
       <c r="G67" s="15"/>
       <c r="H67" s="15"/>
       <c r="I67" s="16"/>
     </row>
-    <row r="68" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="16">
-        <v>907</v>
-      </c>
-      <c r="B68" s="17">
-        <v>45640</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" s="16">
-        <v>2</v>
-      </c>
-      <c r="F68" s="16">
-        <v>2</v>
-      </c>
+    <row r="68" spans="1:9" ht="19" customHeight="1">
+      <c r="A68" s="1">
+        <v>677</v>
+      </c>
+      <c r="B68" s="2">
+        <v>45639</v>
+      </c>
+      <c r="C68" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
       <c r="G68" s="15"/>
       <c r="H68" s="15"/>
       <c r="I68" s="16"/>
     </row>
-    <row r="69" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="16">
+    <row r="69" spans="1:9" ht="19" customHeight="1">
+      <c r="A69" s="1">
         <v>907</v>
       </c>
-      <c r="B69" s="17">
-        <v>45640</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="18" t="s">
+      <c r="B69" s="2">
+        <v>45639</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
       <c r="G69" s="15"/>
       <c r="H69" s="15"/>
       <c r="I69" s="16"/>
     </row>
-    <row r="70" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="16"/>
-      <c r="B70" s="17"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
+    <row r="70" spans="1:9" ht="19" customHeight="1">
+      <c r="A70" s="30">
+        <v>880</v>
+      </c>
+      <c r="B70" s="31">
+        <v>45667</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" s="30">
+        <v>3</v>
+      </c>
+      <c r="F70" s="30">
+        <v>3</v>
+      </c>
       <c r="G70" s="15"/>
       <c r="H70" s="15"/>
       <c r="I70" s="16"/>
     </row>
-    <row r="71" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="16"/>
-      <c r="B71" s="17"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
+    <row r="71" spans="1:9" ht="19" customHeight="1">
+      <c r="A71" s="30">
+        <v>880</v>
+      </c>
+      <c r="B71" s="31">
+        <v>45667</v>
+      </c>
+      <c r="C71" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
       <c r="G71" s="15"/>
       <c r="H71" s="15"/>
       <c r="I71" s="16"/>
     </row>
-    <row r="72" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="16"/>
-      <c r="B72" s="17"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
+    <row r="72" spans="1:9" ht="19" customHeight="1">
+      <c r="A72" s="30">
+        <v>880</v>
+      </c>
+      <c r="B72" s="31">
+        <v>45667</v>
+      </c>
+      <c r="C72" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" s="30"/>
+      <c r="F72" s="30"/>
       <c r="G72" s="15"/>
       <c r="H72" s="15"/>
       <c r="I72" s="16"/>
     </row>
-    <row r="73" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="16"/>
-      <c r="B73" s="17"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
+    <row r="73" spans="1:9" ht="19" customHeight="1">
+      <c r="A73" s="22">
+        <v>843</v>
+      </c>
+      <c r="B73" s="31">
+        <v>45667</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
       <c r="G73" s="15"/>
       <c r="H73" s="15"/>
       <c r="I73" s="16"/>
     </row>
-    <row r="74" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="19" customHeight="1">
       <c r="A74" s="16"/>
       <c r="B74" s="17"/>
       <c r="E74" s="16"/>
@@ -2128,7 +2196,7 @@
       <c r="H74" s="15"/>
       <c r="I74" s="16"/>
     </row>
-    <row r="75" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="19" customHeight="1">
       <c r="A75" s="16"/>
       <c r="B75" s="17"/>
       <c r="E75" s="16"/>
@@ -2137,7 +2205,7 @@
       <c r="H75" s="15"/>
       <c r="I75" s="16"/>
     </row>
-    <row r="76" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="19" customHeight="1">
       <c r="A76" s="16"/>
       <c r="B76" s="17"/>
       <c r="E76" s="16"/>
@@ -2146,7 +2214,7 @@
       <c r="H76" s="15"/>
       <c r="I76" s="16"/>
     </row>
-    <row r="77" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="19" customHeight="1">
       <c r="A77" s="16"/>
       <c r="B77" s="17"/>
       <c r="E77" s="16"/>
@@ -2155,7 +2223,7 @@
       <c r="H77" s="15"/>
       <c r="I77" s="16"/>
     </row>
-    <row r="78" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="19" customHeight="1">
       <c r="A78" s="16"/>
       <c r="B78" s="17"/>
       <c r="E78" s="16"/>
@@ -2164,7 +2232,7 @@
       <c r="H78" s="15"/>
       <c r="I78" s="16"/>
     </row>
-    <row r="79" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="19" customHeight="1">
       <c r="A79" s="16"/>
       <c r="B79" s="17"/>
       <c r="E79" s="16"/>
@@ -2173,8 +2241,14 @@
       <c r="H79" s="15"/>
       <c r="I79" s="16"/>
     </row>
-    <row r="1048576" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1048576" s="17"/>
+    <row r="80" spans="1:9" ht="19" customHeight="1">
+      <c r="A80" s="16"/>
+      <c r="B80" s="17"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gérer les actions float ou int + maj actions 3e série
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zarka/Documents/Simon/Squash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Travail\Personnel\Squash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790EA30D-B462-BE4B-8895-66216923CBBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0E1983-FB92-45A7-80C7-F122EE77ED85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="1760" windowWidth="32620" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions Simon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -149,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,10 +199,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri (Corps)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -349,15 +358,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -667,23 +667,23 @@
   </sheetPr>
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.44140625" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -712,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>6277</v>
       </c>
@@ -744,7 +744,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1">
+    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>7104</v>
       </c>
@@ -769,7 +769,7 @@
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>6332</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>5971</v>
       </c>
@@ -811,7 +811,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="19.5" customHeight="1">
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>7104</v>
       </c>
@@ -830,7 +830,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:9" ht="19.5" customHeight="1">
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6483</v>
       </c>
@@ -849,7 +849,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" ht="19.5" customHeight="1">
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>4919</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
     </row>
-    <row r="9" spans="1:9" ht="19.5" customHeight="1">
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>7191</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="1:9" ht="19.5" customHeight="1">
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>5564</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="H10" s="15"/>
       <c r="I10" s="16"/>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>7191</v>
       </c>
@@ -933,7 +933,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>7191</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="H12" s="15"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>5564</v>
       </c>
@@ -971,7 +971,7 @@
       <c r="H13" s="15"/>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="1:9" ht="19.5" customHeight="1">
+    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>6639</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="H14" s="15"/>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="1:9" ht="19.5" customHeight="1">
+    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>7191</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="1:9" ht="19.5" customHeight="1">
+    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>7155</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="1:9" ht="19.5" customHeight="1">
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>4213</v>
       </c>
@@ -1051,7 +1051,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1">
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1802</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="H18" s="15"/>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" ht="19.5" customHeight="1">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>3347</v>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="H19" s="15"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1">
+    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>2298</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H20" s="15"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:9" ht="19.5" customHeight="1">
+    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>3293</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="H21" s="15"/>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:9" ht="19.5" customHeight="1">
+    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>2082</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="H22" s="15"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" ht="19.5" customHeight="1">
+    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>5063</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="H23" s="15"/>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="1:9" ht="19.5" customHeight="1">
+    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>2910</v>
       </c>
@@ -1196,7 +1196,7 @@
       <c r="H24" s="15"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" ht="19" customHeight="1">
+    <row r="25" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>2484</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="H25" s="15"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:9" ht="19" customHeight="1">
+    <row r="26" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>3071</v>
       </c>
@@ -1234,7 +1234,7 @@
       <c r="H26" s="15"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:9" ht="19" customHeight="1">
+    <row r="27" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>2687</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="H27" s="15"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9" ht="19" customHeight="1">
+    <row r="28" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>2709</v>
       </c>
@@ -1276,7 +1276,7 @@
       <c r="H28" s="15"/>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" ht="19" customHeight="1">
+    <row r="29" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>3457</v>
       </c>
@@ -1295,7 +1295,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:9" ht="19" customHeight="1">
+    <row r="30" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>4288</v>
       </c>
@@ -1314,7 +1314,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" ht="19" customHeight="1">
+    <row r="31" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>3457</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" ht="19" customHeight="1">
+    <row r="32" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>3480</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:9" ht="19" customHeight="1">
+    <row r="33" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>2169</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="16"/>
     </row>
-    <row r="34" spans="1:9" ht="19" customHeight="1">
+    <row r="34" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>2184</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="16"/>
     </row>
-    <row r="35" spans="1:9" ht="19.5" customHeight="1">
+    <row r="35" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>4288</v>
       </c>
@@ -1417,7 +1417,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="16"/>
     </row>
-    <row r="36" spans="1:9" ht="19.5" customHeight="1">
+    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>3763</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="H36" s="15"/>
       <c r="I36" s="16"/>
     </row>
-    <row r="37" spans="1:9" ht="19.5" customHeight="1">
+    <row r="37" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>4288</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="H37" s="15"/>
       <c r="I37" s="16"/>
     </row>
-    <row r="38" spans="1:9" ht="19.5" customHeight="1">
+    <row r="38" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>2015</v>
       </c>
@@ -1478,7 +1478,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="16"/>
     </row>
-    <row r="39" spans="1:9" ht="19.5" customHeight="1">
+    <row r="39" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>1814</v>
       </c>
@@ -1497,7 +1497,7 @@
       <c r="H39" s="15"/>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:9" ht="19.5" customHeight="1">
+    <row r="40" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>1829</v>
       </c>
@@ -1516,7 +1516,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="16"/>
     </row>
-    <row r="41" spans="1:9" ht="19.5" customHeight="1">
+    <row r="41" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>1387</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="16"/>
     </row>
-    <row r="42" spans="1:9" ht="19.5" customHeight="1">
+    <row r="42" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>1321</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:9" ht="19.5" customHeight="1">
+    <row r="43" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>1772</v>
       </c>
@@ -1577,7 +1577,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="16"/>
     </row>
-    <row r="44" spans="1:9" ht="20.25" customHeight="1">
+    <row r="44" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>1280</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="16"/>
     </row>
-    <row r="45" spans="1:9" ht="20.25" customHeight="1">
+    <row r="45" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2081</v>
       </c>
@@ -1619,7 +1619,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:9" ht="20.25" customHeight="1">
+    <row r="46" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2049</v>
       </c>
@@ -1638,7 +1638,7 @@
       <c r="H46" s="15"/>
       <c r="I46" s="16"/>
     </row>
-    <row r="47" spans="1:9" ht="19.5" customHeight="1">
+    <row r="47" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2081</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="16"/>
     </row>
-    <row r="48" spans="1:9" ht="19.5" customHeight="1">
+    <row r="48" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>1296</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" ht="19.5" customHeight="1">
+    <row r="49" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2049</v>
       </c>
@@ -1703,7 +1703,7 @@
       <c r="H49" s="15"/>
       <c r="I49" s="16"/>
     </row>
-    <row r="50" spans="1:9" ht="19.5" customHeight="1">
+    <row r="50" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>1676</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="H50" s="15"/>
       <c r="I50" s="16"/>
     </row>
-    <row r="51" spans="1:9" ht="19.5" customHeight="1">
+    <row r="51" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22">
         <v>2081</v>
       </c>
@@ -1745,7 +1745,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="16"/>
     </row>
-    <row r="52" spans="1:9" ht="19.5" customHeight="1">
+    <row r="52" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22">
         <v>1970</v>
       </c>
@@ -1764,7 +1764,7 @@
       <c r="H52" s="15"/>
       <c r="I52" s="16"/>
     </row>
-    <row r="53" spans="1:9" ht="19.5" customHeight="1">
+    <row r="53" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="22">
         <v>476</v>
       </c>
@@ -1787,7 +1787,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" ht="19.5" customHeight="1">
+    <row r="54" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="22">
         <v>1501</v>
       </c>
@@ -1806,7 +1806,7 @@
       <c r="H54" s="15"/>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" ht="19" customHeight="1">
+    <row r="55" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="22">
         <v>476</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="H55" s="15"/>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:9" ht="19" customHeight="1">
+    <row r="56" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>451</v>
       </c>
@@ -1848,7 +1848,7 @@
       <c r="H56" s="15"/>
       <c r="I56" s="16"/>
     </row>
-    <row r="57" spans="1:9" ht="19" customHeight="1">
+    <row r="57" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>682</v>
       </c>
@@ -1867,7 +1867,7 @@
       <c r="H57" s="15"/>
       <c r="I57" s="16"/>
     </row>
-    <row r="58" spans="1:9" ht="19" customHeight="1">
+    <row r="58" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>535</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="H58" s="15"/>
       <c r="I58" s="16"/>
     </row>
-    <row r="59" spans="1:9" ht="19" customHeight="1">
+    <row r="59" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>641</v>
       </c>
@@ -1905,7 +1905,7 @@
       <c r="H59" s="15"/>
       <c r="I59" s="16"/>
     </row>
-    <row r="60" spans="1:9" ht="19" customHeight="1">
+    <row r="60" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="27">
         <v>1171</v>
       </c>
@@ -1928,7 +1928,7 @@
       <c r="H60" s="15"/>
       <c r="I60" s="16"/>
     </row>
-    <row r="61" spans="1:9" ht="19" customHeight="1">
+    <row r="61" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="27">
         <v>1197</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="H61" s="15"/>
       <c r="I61" s="16"/>
     </row>
-    <row r="62" spans="1:9" ht="19" customHeight="1">
+    <row r="62" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="27">
         <v>641</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="H62" s="15"/>
       <c r="I62" s="16"/>
     </row>
-    <row r="63" spans="1:9" ht="19" customHeight="1">
+    <row r="63" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="27">
         <v>641</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="H63" s="15"/>
       <c r="I63" s="16"/>
     </row>
-    <row r="64" spans="1:9" ht="19" customHeight="1">
+    <row r="64" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>1069</v>
       </c>
@@ -2008,7 +2008,7 @@
       <c r="H64" s="15"/>
       <c r="I64" s="16"/>
     </row>
-    <row r="65" spans="1:9" ht="19" customHeight="1">
+    <row r="65" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>1153</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="H65" s="15"/>
       <c r="I65" s="16"/>
     </row>
-    <row r="66" spans="1:9" ht="19" customHeight="1">
+    <row r="66" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>1111</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="H66" s="15"/>
       <c r="I66" s="16"/>
     </row>
-    <row r="67" spans="1:9" ht="19" customHeight="1">
+    <row r="67" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>907</v>
       </c>
@@ -2069,7 +2069,7 @@
       <c r="H67" s="15"/>
       <c r="I67" s="16"/>
     </row>
-    <row r="68" spans="1:9" ht="19" customHeight="1">
+    <row r="68" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>677</v>
       </c>
@@ -2088,7 +2088,7 @@
       <c r="H68" s="15"/>
       <c r="I68" s="16"/>
     </row>
-    <row r="69" spans="1:9" ht="19" customHeight="1">
+    <row r="69" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>907</v>
       </c>
@@ -2107,87 +2107,87 @@
       <c r="H69" s="15"/>
       <c r="I69" s="16"/>
     </row>
-    <row r="70" spans="1:9" ht="19" customHeight="1">
-      <c r="A70" s="30">
+    <row r="70" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="27">
         <v>880</v>
       </c>
-      <c r="B70" s="31">
+      <c r="B70" s="28">
         <v>45667</v>
       </c>
-      <c r="C70" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="32" t="s">
+      <c r="C70" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E70" s="30">
+      <c r="E70" s="27">
         <v>3</v>
       </c>
-      <c r="F70" s="30">
+      <c r="F70" s="27">
         <v>3</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="15"/>
       <c r="I70" s="16"/>
     </row>
-    <row r="71" spans="1:9" ht="19" customHeight="1">
-      <c r="A71" s="30">
+    <row r="71" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="27">
         <v>880</v>
       </c>
-      <c r="B71" s="31">
+      <c r="B71" s="28">
         <v>45667</v>
       </c>
-      <c r="C71" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" s="32" t="s">
+      <c r="C71" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
       <c r="G71" s="15"/>
       <c r="H71" s="15"/>
       <c r="I71" s="16"/>
     </row>
-    <row r="72" spans="1:9" ht="19" customHeight="1">
-      <c r="A72" s="30">
+    <row r="72" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="27">
         <v>880</v>
       </c>
-      <c r="B72" s="31">
+      <c r="B72" s="28">
         <v>45667</v>
       </c>
-      <c r="C72" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72" s="32" t="s">
+      <c r="C72" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E72" s="30"/>
-      <c r="F72" s="30"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
       <c r="G72" s="15"/>
       <c r="H72" s="15"/>
       <c r="I72" s="16"/>
     </row>
-    <row r="73" spans="1:9" ht="19" customHeight="1">
-      <c r="A73" s="22">
-        <v>843</v>
-      </c>
-      <c r="B73" s="31">
+    <row r="73" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="27">
+        <v>758.7</v>
+      </c>
+      <c r="B73" s="28">
         <v>45667</v>
       </c>
-      <c r="C73" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="32" t="s">
+      <c r="C73" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
+      <c r="E73" s="27"/>
+      <c r="F73" s="27"/>
       <c r="G73" s="15"/>
       <c r="H73" s="15"/>
       <c r="I73" s="16"/>
     </row>
-    <row r="74" spans="1:9" ht="19" customHeight="1">
+    <row r="74" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="17"/>
       <c r="E74" s="16"/>
@@ -2196,7 +2196,7 @@
       <c r="H74" s="15"/>
       <c r="I74" s="16"/>
     </row>
-    <row r="75" spans="1:9" ht="19" customHeight="1">
+    <row r="75" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="17"/>
       <c r="E75" s="16"/>
@@ -2205,7 +2205,7 @@
       <c r="H75" s="15"/>
       <c r="I75" s="16"/>
     </row>
-    <row r="76" spans="1:9" ht="19" customHeight="1">
+    <row r="76" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="16"/>
       <c r="B76" s="17"/>
       <c r="E76" s="16"/>
@@ -2214,7 +2214,7 @@
       <c r="H76" s="15"/>
       <c r="I76" s="16"/>
     </row>
-    <row r="77" spans="1:9" ht="19" customHeight="1">
+    <row r="77" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
       <c r="B77" s="17"/>
       <c r="E77" s="16"/>
@@ -2223,7 +2223,7 @@
       <c r="H77" s="15"/>
       <c r="I77" s="16"/>
     </row>
-    <row r="78" spans="1:9" ht="19" customHeight="1">
+    <row r="78" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="17"/>
       <c r="E78" s="16"/>
@@ -2232,7 +2232,7 @@
       <c r="H78" s="15"/>
       <c r="I78" s="16"/>
     </row>
-    <row r="79" spans="1:9" ht="19" customHeight="1">
+    <row r="79" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
       <c r="B79" s="17"/>
       <c r="E79" s="16"/>
@@ -2241,7 +2241,7 @@
       <c r="H79" s="15"/>
       <c r="I79" s="16"/>
     </row>
-    <row r="80" spans="1:9" ht="19" customHeight="1">
+    <row r="80" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16"/>
       <c r="B80" s="17"/>
       <c r="E80" s="16"/>

</xml_diff>

<commit_message>
résultats championnat 2eme série
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -1,39 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Travail\Personnel\Squash\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DC506E-BE87-4824-974B-4C247092DE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Actions Simon" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Actions Simon"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="46">
   <si>
     <t>Points</t>
   </si>
@@ -165,16 +146,22 @@
   </si>
   <si>
     <t>Verrières Place</t>
+  </si>
+  <si>
+    <t>2ème Série IDF Place</t>
+  </si>
+  <si>
+    <t>2ème Série IDF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,12 +179,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -264,88 +245,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -356,10 +334,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -397,71 +375,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -489,7 +467,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -512,11 +490,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -525,13 +503,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -541,7 +519,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -550,7 +528,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -559,7 +537,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -567,10 +545,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -635,29 +613,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="19" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="21" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="21" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="22" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="22" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="23" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="23" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="22" width="10.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5">
         <v>6277</v>
       </c>
@@ -707,18 +684,15 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(E:E)</f>
-        <v>64</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>30</v>
       </c>
       <c r="I2" s="5">
         <f>SUM(G2:H2)</f>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="5">
         <v>7104</v>
       </c>
@@ -735,15 +709,13 @@
       <c r="F3" s="5"/>
       <c r="G3" s="8">
         <f>G2/I2</f>
-        <v>0.68085106382978722</v>
       </c>
       <c r="H3" s="8">
         <f>H2/I2</f>
-        <v>0.31914893617021278</v>
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5">
         <v>6332</v>
       </c>
@@ -762,7 +734,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5">
         <v>5971</v>
       </c>
@@ -785,7 +757,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5">
         <v>7104</v>
       </c>
@@ -804,7 +776,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5">
         <v>6483</v>
       </c>
@@ -823,7 +795,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5">
         <v>4919</v>
       </c>
@@ -846,7 +818,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5">
         <v>7191</v>
       </c>
@@ -865,7 +837,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5">
         <v>5564</v>
       </c>
@@ -888,7 +860,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5">
         <v>7191</v>
       </c>
@@ -907,7 +879,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5">
         <v>7191</v>
       </c>
@@ -926,7 +898,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5">
         <v>5564</v>
       </c>
@@ -945,7 +917,7 @@
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5">
         <v>6639</v>
       </c>
@@ -968,7 +940,7 @@
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5">
         <v>7191</v>
       </c>
@@ -987,7 +959,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5">
         <v>7155</v>
       </c>
@@ -1006,7 +978,7 @@
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5">
         <v>4213</v>
       </c>
@@ -1025,7 +997,7 @@
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5">
         <v>1802</v>
       </c>
@@ -1048,7 +1020,7 @@
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5">
         <v>3347</v>
       </c>
@@ -1071,7 +1043,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5">
         <v>2298</v>
       </c>
@@ -1090,7 +1062,7 @@
       <c r="H20" s="9"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="5">
         <v>3293</v>
       </c>
@@ -1109,7 +1081,7 @@
       <c r="H21" s="9"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="5">
         <v>2082</v>
       </c>
@@ -1128,7 +1100,7 @@
       <c r="H22" s="9"/>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="5">
         <v>5063</v>
       </c>
@@ -1147,7 +1119,7 @@
       <c r="H23" s="9"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="5">
         <v>2910</v>
       </c>
@@ -1170,7 +1142,7 @@
       <c r="H24" s="9"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.05">
       <c r="A25" s="5">
         <v>2484</v>
       </c>
@@ -1189,7 +1161,7 @@
       <c r="H25" s="9"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.05">
       <c r="A26" s="5">
         <v>3071</v>
       </c>
@@ -1208,7 +1180,7 @@
       <c r="H26" s="9"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.05">
       <c r="A27" s="5">
         <v>2687</v>
       </c>
@@ -1227,7 +1199,7 @@
       <c r="H27" s="9"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.05">
       <c r="A28" s="5">
         <v>2709</v>
       </c>
@@ -1250,7 +1222,7 @@
       <c r="H28" s="9"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.05">
       <c r="A29" s="5">
         <v>3457</v>
       </c>
@@ -1269,7 +1241,7 @@
       <c r="H29" s="9"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.05">
       <c r="A30" s="5">
         <v>4288</v>
       </c>
@@ -1288,7 +1260,7 @@
       <c r="H30" s="9"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.05">
       <c r="A31" s="5">
         <v>3457</v>
       </c>
@@ -1307,7 +1279,7 @@
       <c r="H31" s="9"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.05">
       <c r="A32" s="5">
         <v>3480</v>
       </c>
@@ -1330,7 +1302,7 @@
       <c r="H32" s="9"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.05">
       <c r="A33" s="5">
         <v>2169</v>
       </c>
@@ -1349,7 +1321,7 @@
       <c r="H33" s="9"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.05">
       <c r="A34" s="5">
         <v>2184</v>
       </c>
@@ -1368,7 +1340,7 @@
       <c r="H34" s="9"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="5">
         <v>4288</v>
       </c>
@@ -1391,7 +1363,7 @@
       <c r="H35" s="9"/>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="5">
         <v>3763</v>
       </c>
@@ -1410,7 +1382,7 @@
       <c r="H36" s="9"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="5">
         <v>4288</v>
       </c>
@@ -1429,7 +1401,7 @@
       <c r="H37" s="9"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="5">
         <v>2015</v>
       </c>
@@ -1452,7 +1424,7 @@
       <c r="H38" s="9"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="5">
         <v>1814</v>
       </c>
@@ -1471,7 +1443,7 @@
       <c r="H39" s="9"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="5">
         <v>1829</v>
       </c>
@@ -1490,7 +1462,7 @@
       <c r="H40" s="9"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="5">
         <v>1387</v>
       </c>
@@ -1513,7 +1485,7 @@
       <c r="H41" s="9"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="5">
         <v>1321</v>
       </c>
@@ -1532,7 +1504,7 @@
       <c r="H42" s="9"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="5">
         <v>1772</v>
       </c>
@@ -1551,7 +1523,7 @@
       <c r="H43" s="9"/>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
       <c r="A44" s="11">
         <v>1280</v>
       </c>
@@ -1570,7 +1542,7 @@
       <c r="H44" s="9"/>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
       <c r="A45" s="5">
         <v>2081</v>
       </c>
@@ -1593,7 +1565,7 @@
       <c r="H45" s="9"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
       <c r="A46" s="5">
         <v>2049</v>
       </c>
@@ -1612,7 +1584,7 @@
       <c r="H46" s="9"/>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="5">
         <v>2081</v>
       </c>
@@ -1635,7 +1607,7 @@
       <c r="H47" s="9"/>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="5">
         <v>1296</v>
       </c>
@@ -1658,7 +1630,7 @@
       <c r="H48" s="9"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="5">
         <v>2049</v>
       </c>
@@ -1677,7 +1649,7 @@
       <c r="H49" s="9"/>
       <c r="I49" s="10"/>
     </row>
-    <row r="50" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="5">
         <v>1676</v>
       </c>
@@ -1696,120 +1668,120 @@
       <c r="H50" s="9"/>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="14">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+      <c r="A51" s="5">
         <v>2081</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="6">
         <v>45591</v>
       </c>
-      <c r="C51" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="16" t="s">
+      <c r="C51" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="5">
         <v>4</v>
       </c>
-      <c r="F51" s="14">
+      <c r="F51" s="5">
         <v>0</v>
       </c>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
       <c r="I51" s="10"/>
     </row>
-    <row r="52" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="14">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+      <c r="A52" s="5">
         <v>1970</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="6">
         <v>45594</v>
       </c>
-      <c r="C52" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
       <c r="I52" s="10"/>
     </row>
-    <row r="53" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="14">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+      <c r="A53" s="5">
         <v>476</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="6">
         <v>45598</v>
       </c>
-      <c r="C53" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="16" t="s">
+      <c r="C53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E53" s="5">
         <v>4</v>
       </c>
-      <c r="F53" s="14">
+      <c r="F53" s="5">
         <v>1</v>
       </c>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="14">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+      <c r="A54" s="5">
         <v>1501</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="6">
         <v>45598</v>
       </c>
-      <c r="C54" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="16" t="s">
+      <c r="C54" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="14">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.05">
+      <c r="A55" s="5">
         <v>476</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="6">
         <v>45598</v>
       </c>
-      <c r="C55" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="16" t="s">
+      <c r="C55" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="10"/>
     </row>
-    <row r="56" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.05">
       <c r="A56" s="5">
         <v>451</v>
       </c>
       <c r="B56" s="6">
         <v>45612</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="17" t="s">
+      <c r="C56" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E56" s="5">
@@ -1822,17 +1794,17 @@
       <c r="H56" s="9"/>
       <c r="I56" s="10"/>
     </row>
-    <row r="57" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.05">
       <c r="A57" s="5">
         <v>682</v>
       </c>
       <c r="B57" s="6">
         <v>45612</v>
       </c>
-      <c r="C57" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="17" t="s">
+      <c r="C57" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E57" s="5"/>
@@ -1841,17 +1813,17 @@
       <c r="H57" s="9"/>
       <c r="I57" s="10"/>
     </row>
-    <row r="58" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.05">
       <c r="A58" s="5">
         <v>535</v>
       </c>
       <c r="B58" s="6">
         <v>45612</v>
       </c>
-      <c r="C58" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="17" t="s">
+      <c r="C58" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E58" s="5"/>
@@ -1860,17 +1832,17 @@
       <c r="H58" s="9"/>
       <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="5">
         <v>641</v>
       </c>
       <c r="B59" s="6">
         <v>45612</v>
       </c>
-      <c r="C59" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="17" t="s">
+      <c r="C59" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E59" s="5"/>
@@ -1879,97 +1851,97 @@
       <c r="H59" s="9"/>
       <c r="I59" s="10"/>
     </row>
-    <row r="60" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="14">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+      <c r="A60" s="5">
         <v>1171</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="6">
         <v>45618</v>
       </c>
-      <c r="C60" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="16" t="s">
+      <c r="C60" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="14">
+      <c r="E60" s="5">
         <v>5</v>
       </c>
-      <c r="F60" s="14">
+      <c r="F60" s="5">
         <v>0</v>
       </c>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
       <c r="I60" s="10"/>
     </row>
-    <row r="61" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="14">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+      <c r="A61" s="5">
         <v>1197</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="6">
         <v>45618</v>
       </c>
-      <c r="C61" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" s="16" t="s">
+      <c r="C61" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
       <c r="I61" s="10"/>
     </row>
-    <row r="62" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="14">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+      <c r="A62" s="5">
         <v>641</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="6">
         <v>45618</v>
       </c>
-      <c r="C62" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="16" t="s">
+      <c r="C62" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
       <c r="I62" s="10"/>
     </row>
-    <row r="63" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="14">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+      <c r="A63" s="5">
         <v>641</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="6">
         <v>45618</v>
       </c>
-      <c r="C63" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="16" t="s">
+      <c r="C63" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
       <c r="I63" s="10"/>
     </row>
-    <row r="64" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="5">
         <v>1069</v>
       </c>
       <c r="B64" s="6">
         <v>45626</v>
       </c>
-      <c r="C64" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" s="17" t="s">
+      <c r="C64" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E64" s="5">
@@ -1982,17 +1954,17 @@
       <c r="H64" s="9"/>
       <c r="I64" s="10"/>
     </row>
-    <row r="65" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="5">
         <v>1153</v>
       </c>
       <c r="B65" s="6">
         <v>45626</v>
       </c>
-      <c r="C65" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65" s="17" t="s">
+      <c r="C65" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E65" s="5"/>
@@ -2001,17 +1973,17 @@
       <c r="H65" s="9"/>
       <c r="I65" s="10"/>
     </row>
-    <row r="66" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="5">
         <v>1111</v>
       </c>
       <c r="B66" s="6">
         <v>45626</v>
       </c>
-      <c r="C66" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" s="17" t="s">
+      <c r="C66" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E66" s="5"/>
@@ -2020,17 +1992,17 @@
       <c r="H66" s="9"/>
       <c r="I66" s="10"/>
     </row>
-    <row r="67" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="5">
         <v>907</v>
       </c>
       <c r="B67" s="6">
         <v>45639</v>
       </c>
-      <c r="C67" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" s="17" t="s">
+      <c r="C67" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E67" s="5">
@@ -2043,17 +2015,17 @@
       <c r="H67" s="9"/>
       <c r="I67" s="10"/>
     </row>
-    <row r="68" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="5">
         <v>677</v>
       </c>
       <c r="B68" s="6">
         <v>45639</v>
       </c>
-      <c r="C68" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" s="17" t="s">
+      <c r="C68" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E68" s="5"/>
@@ -2062,17 +2034,17 @@
       <c r="H68" s="9"/>
       <c r="I68" s="10"/>
     </row>
-    <row r="69" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="5">
         <v>907</v>
       </c>
       <c r="B69" s="6">
         <v>45639</v>
       </c>
-      <c r="C69" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="17" t="s">
+      <c r="C69" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E69" s="5"/>
@@ -2081,97 +2053,97 @@
       <c r="H69" s="9"/>
       <c r="I69" s="10"/>
     </row>
-    <row r="70" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="14">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+      <c r="A70" s="5">
         <v>880</v>
       </c>
-      <c r="B70" s="15">
+      <c r="B70" s="6">
         <v>45667</v>
       </c>
-      <c r="C70" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="16" t="s">
+      <c r="C70" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E70" s="14">
+      <c r="E70" s="5">
         <v>3</v>
       </c>
-      <c r="F70" s="14">
+      <c r="F70" s="5">
         <v>3</v>
       </c>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
       <c r="I70" s="10"/>
     </row>
-    <row r="71" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="14">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+      <c r="A71" s="5">
         <v>880</v>
       </c>
-      <c r="B71" s="15">
+      <c r="B71" s="6">
         <v>45667</v>
       </c>
-      <c r="C71" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" s="16" t="s">
+      <c r="C71" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
       <c r="I71" s="10"/>
     </row>
-    <row r="72" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="14">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
+      <c r="A72" s="5">
         <v>880</v>
       </c>
-      <c r="B72" s="15">
+      <c r="B72" s="6">
         <v>45667</v>
       </c>
-      <c r="C72" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72" s="16" t="s">
+      <c r="C72" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
       <c r="I72" s="10"/>
     </row>
-    <row r="73" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="14">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="20.25">
+      <c r="A73" s="5">
         <v>758.7</v>
       </c>
-      <c r="B73" s="15">
+      <c r="B73" s="6">
         <v>45667</v>
       </c>
-      <c r="C73" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="16" t="s">
+      <c r="C73" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
       <c r="I73" s="10"/>
     </row>
-    <row r="74" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="10">
         <v>880</v>
       </c>
-      <c r="B74" s="18">
+      <c r="B74" s="14">
         <v>45673</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D74" s="19" t="s">
+      <c r="D74" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E74" s="10">
@@ -2184,17 +2156,17 @@
       <c r="H74" s="9"/>
       <c r="I74" s="10"/>
     </row>
-    <row r="75" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="10">
         <v>880</v>
       </c>
-      <c r="B75" s="18">
+      <c r="B75" s="14">
         <v>45676</v>
       </c>
-      <c r="C75" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D75" s="23" t="s">
+      <c r="C75" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="15" t="s">
         <v>42</v>
       </c>
       <c r="E75" s="10"/>
@@ -2203,17 +2175,17 @@
       <c r="H75" s="9"/>
       <c r="I75" s="10"/>
     </row>
-    <row r="76" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="10">
         <v>880</v>
       </c>
-      <c r="B76" s="18">
+      <c r="B76" s="14">
         <v>45676</v>
       </c>
-      <c r="C76" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D76" s="23" t="s">
+      <c r="C76" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="15" t="s">
         <v>42</v>
       </c>
       <c r="E76" s="10"/>
@@ -2222,17 +2194,17 @@
       <c r="H76" s="9"/>
       <c r="I76" s="10"/>
     </row>
-    <row r="77" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="10">
         <v>801</v>
       </c>
-      <c r="B77" s="18">
+      <c r="B77" s="14">
         <v>45676</v>
       </c>
-      <c r="C77" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77" s="23" t="s">
+      <c r="C77" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="15" t="s">
         <v>42</v>
       </c>
       <c r="E77" s="10"/>
@@ -2241,17 +2213,17 @@
       <c r="H77" s="9"/>
       <c r="I77" s="10"/>
     </row>
-    <row r="78" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="10">
         <v>879</v>
       </c>
-      <c r="B78" s="18">
+      <c r="B78" s="14">
         <v>45676</v>
       </c>
-      <c r="C78" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D78" s="23" t="s">
+      <c r="C78" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E78" s="10">
@@ -2264,24 +2236,67 @@
       <c r="H78" s="9"/>
       <c r="I78" s="10"/>
     </row>
-    <row r="79" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="10"/>
-      <c r="B79" s="18"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
+      <c r="A79" s="10">
+        <v>538.2</v>
+      </c>
+      <c r="B79" s="14">
+        <v>45725</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" s="10">
+        <v>4</v>
+      </c>
+      <c r="F79" s="10">
+        <v>2</v>
+      </c>
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
       <c r="I79" s="10"/>
     </row>
-    <row r="80" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="10"/>
-      <c r="B80" s="18"/>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
+      <c r="A80" s="10">
+        <v>464</v>
+      </c>
+      <c r="B80" s="14">
+        <v>45725</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="E80" s="10"/>
       <c r="F80" s="10"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
       <c r="I80" s="10"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+      <c r="A81" s="16">
+        <v>598</v>
+      </c>
+      <c r="B81" s="14">
+        <v>45725</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="17"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update correspondance points - rang
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Travail\Personnel\Squash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16927F80-8B22-4D41-9772-2C74ECA9A419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4BE407-CC8B-4466-BDA3-E2D404363580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions Simon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="51">
   <si>
     <t>Points</t>
   </si>
@@ -180,6 +167,12 @@
   </si>
   <si>
     <t>PUC Place</t>
+  </si>
+  <si>
+    <t>UCPA Paris 19</t>
+  </si>
+  <si>
+    <t>National Squash 95</t>
   </si>
 </sst>
 </file>
@@ -638,10 +631,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,15 +699,15 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(E:E)</f>
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="I2" s="5">
         <f>SUM(G2:H2)</f>
-        <v>109</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -734,11 +727,11 @@
       <c r="F3" s="5"/>
       <c r="G3" s="8">
         <f>G2/I2</f>
-        <v>0.66972477064220182</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="H3" s="8">
         <f>H2/I2</f>
-        <v>0.33027522935779818</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="I3" s="5"/>
     </row>
@@ -2426,12 +2419,208 @@
       <c r="F87" s="19"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
+      <c r="A88" s="19">
+        <v>528</v>
+      </c>
+      <c r="B88" s="20">
+        <v>45816</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E88" s="19">
+        <v>2</v>
+      </c>
+      <c r="F88" s="19">
+        <v>3</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="19">
+        <v>329</v>
+      </c>
+      <c r="B89" s="20">
+        <v>45816</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="E89" s="19"/>
       <c r="F89" s="19"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="19">
+        <v>421</v>
+      </c>
+      <c r="B90" s="20">
+        <v>45816</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="19">
+        <v>557</v>
+      </c>
+      <c r="B91" s="20">
+        <v>45829</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E91" s="19">
+        <v>2</v>
+      </c>
+      <c r="F91" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="19">
+        <v>419</v>
+      </c>
+      <c r="B92" s="20">
+        <v>45829</v>
+      </c>
+      <c r="C92" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="19">
+        <v>515</v>
+      </c>
+      <c r="B93" s="20">
+        <v>45829</v>
+      </c>
+      <c r="C93" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="19">
+        <v>419</v>
+      </c>
+      <c r="B94" s="20">
+        <v>45836</v>
+      </c>
+      <c r="C94" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E94" s="19">
+        <v>2</v>
+      </c>
+      <c r="F94" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="19">
+        <v>557</v>
+      </c>
+      <c r="B95" s="20">
+        <v>45836</v>
+      </c>
+      <c r="C95" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="19">
+        <v>516</v>
+      </c>
+      <c r="B96" s="20">
+        <v>45836</v>
+      </c>
+      <c r="C96" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="19">
+        <v>416</v>
+      </c>
+      <c r="B97" s="20">
+        <v>45843</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" s="19">
+        <v>2</v>
+      </c>
+      <c r="F97" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="19">
+        <v>416</v>
+      </c>
+      <c r="B98" s="20">
+        <v>45843</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="19">
+        <v>476</v>
+      </c>
+      <c r="B99" s="20">
+        <v>45843</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" s="21" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ajout tournoi Jeu de Paume
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galadrim/Documents/perso/Squash-Data/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zarka/Documents/Simon/Squash/Squash-Data/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C951575-ABF5-8047-9FA2-E6931C19C0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83565E53-71E4-F344-987A-4FF25ADA4BCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions Simon" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="181">
   <si>
     <t>Points</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>SF Place</t>
+  </si>
+  <si>
+    <t>Jeu de Paume</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -600,7 +603,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3172,6 +3175,26 @@
         <v>38</v>
       </c>
     </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>161</v>
+      </c>
+      <c r="B132" s="1">
+        <v>46047</v>
+      </c>
+      <c r="C132" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" t="s">
+        <v>180</v>
+      </c>
+      <c r="E132">
+        <v>2</v>
+      </c>
+      <c r="F132">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Ajoput 3ème série IdF
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zarka/Documents/Simon/Squash/Squash-Data/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83565E53-71E4-F344-987A-4FF25ADA4BCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7477BAF8-5136-9441-963B-87616C34B712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="181">
   <si>
     <t>Points</t>
   </si>
@@ -601,9 +601,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,34 +948,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="111" workbookViewId="0">
+      <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -984,22 +993,22 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>45538</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
@@ -1013,16 +1022,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>45538</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G3" t="s">
@@ -1033,16 +1042,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>45538</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G4" t="s">
@@ -1050,22 +1059,22 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>45371</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G5" t="s">
@@ -1079,16 +1088,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>45371</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
@@ -1102,16 +1111,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>45371</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G7" t="s">
@@ -1122,22 +1131,22 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>45395</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
@@ -1145,16 +1154,16 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>45395</v>
       </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G9" t="s">
@@ -1168,22 +1177,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>45406</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G10" t="s">
@@ -1197,16 +1206,16 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>45406</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
@@ -1217,1982 +1226,2016 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>45406</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>45406</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>45387</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>45387</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>45387</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>45387</v>
       </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>45427</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>45297</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>45297</v>
       </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>45297</v>
       </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>45297</v>
       </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>45418</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>45510</v>
       </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>45510</v>
       </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>45510</v>
       </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>45510</v>
       </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>45465</v>
       </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>45465</v>
       </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>45465</v>
       </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>45465</v>
       </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>45468</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>45468</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>45468</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>45472</v>
       </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>45472</v>
       </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>45472</v>
       </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>45419</v>
       </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>45419</v>
       </c>
-      <c r="C39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>45419</v>
       </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>45535</v>
       </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>45300</v>
       </c>
-      <c r="C42" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>45300</v>
       </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>45300</v>
       </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>45453</v>
       </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E45" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>45453</v>
       </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>45606</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>45578</v>
       </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E48" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>45578</v>
       </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>45578</v>
       </c>
-      <c r="C50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>45591</v>
       </c>
-      <c r="C51" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>45591</v>
       </c>
-      <c r="C52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>45333</v>
       </c>
-      <c r="C53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>45333</v>
       </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>45333</v>
       </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>45612</v>
       </c>
-      <c r="C56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="C56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="2">
         <v>45612</v>
       </c>
-      <c r="C57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="C57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="2">
         <v>45612</v>
       </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="2">
         <v>45612</v>
       </c>
-      <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="2">
         <v>45618</v>
       </c>
-      <c r="C60" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="C60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="2">
         <v>45618</v>
       </c>
-      <c r="C61" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="2">
         <v>45618</v>
       </c>
-      <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="C62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="2">
         <v>45618</v>
       </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="C63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="2">
         <v>45626</v>
       </c>
-      <c r="C64" t="s">
-        <v>10</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="C64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E64" t="s">
-        <v>12</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="2">
         <v>45626</v>
       </c>
-      <c r="C65" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="C65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="2">
         <v>45626</v>
       </c>
-      <c r="C66" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="C66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="2">
         <v>45639</v>
       </c>
-      <c r="C67" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="C67" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E67" t="s">
-        <v>12</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="2">
         <v>45639</v>
       </c>
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="C68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="2">
         <v>45639</v>
       </c>
-      <c r="C69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
         <v>45931</v>
       </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="C70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="2">
         <v>45931</v>
       </c>
-      <c r="C71" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="C71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="2">
         <v>45931</v>
       </c>
-      <c r="C72" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="2">
         <v>45931</v>
       </c>
-      <c r="C73" t="s">
-        <v>10</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="2">
         <v>45673</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="A75" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="2">
         <v>45676</v>
       </c>
-      <c r="C75" t="s">
-        <v>10</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="C75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
         <v>45676</v>
       </c>
-      <c r="C76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="C76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="2">
         <v>45676</v>
       </c>
-      <c r="C77" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="C77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="2">
         <v>45676</v>
       </c>
-      <c r="C78" t="s">
-        <v>10</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="A79" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="2">
         <v>45872</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="A80" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="2">
         <v>45872</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="A81" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="2">
         <v>45872</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
         <v>45731</v>
       </c>
-      <c r="C82" t="s">
-        <v>10</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="C82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E82" t="s">
-        <v>12</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="E82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="2">
         <v>45731</v>
       </c>
-      <c r="C83" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="C83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="A84" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="2">
         <v>45731</v>
       </c>
-      <c r="C84" t="s">
-        <v>10</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="C84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="2">
         <v>45731</v>
       </c>
-      <c r="C85" t="s">
-        <v>10</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="C85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="2">
         <v>45721</v>
       </c>
-      <c r="C86" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E86" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="2">
         <v>45721</v>
       </c>
-      <c r="C87" t="s">
-        <v>10</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="2">
         <v>45721</v>
       </c>
-      <c r="C88" t="s">
-        <v>10</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="C88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="2">
         <v>45875</v>
       </c>
-      <c r="C89" t="s">
-        <v>10</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E89" t="s">
-        <v>12</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="2">
         <v>45875</v>
       </c>
-      <c r="C90" t="s">
-        <v>10</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="C90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="2">
         <v>45875</v>
       </c>
-      <c r="C91" t="s">
-        <v>10</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="C91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="2">
         <v>45829</v>
       </c>
-      <c r="C92" t="s">
-        <v>10</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="C92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E92" t="s">
-        <v>12</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="2">
         <v>45829</v>
       </c>
-      <c r="C93" t="s">
-        <v>10</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="C93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="2">
         <v>45829</v>
       </c>
-      <c r="C94" t="s">
-        <v>10</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="C94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="2">
         <v>45835</v>
       </c>
-      <c r="C95" t="s">
-        <v>10</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="C95" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E95" t="s">
-        <v>12</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="2">
         <v>45835</v>
       </c>
-      <c r="C96" t="s">
-        <v>10</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="C96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="2">
         <v>45835</v>
       </c>
-      <c r="C97" t="s">
-        <v>10</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="2">
         <v>45784</v>
       </c>
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E98" t="s">
-        <v>12</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="2">
         <v>45784</v>
       </c>
-      <c r="C99" t="s">
-        <v>10</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="C99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="2">
         <v>45784</v>
       </c>
-      <c r="C100" t="s">
-        <v>10</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="C100" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="2">
         <v>45907</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="A102" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="2">
         <v>45899</v>
       </c>
-      <c r="C102" t="s">
-        <v>10</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="C102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="2">
         <v>45899</v>
       </c>
-      <c r="C103" t="s">
-        <v>10</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="C103" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="A104" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="2">
         <v>45899</v>
       </c>
-      <c r="C104" t="s">
-        <v>10</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="C104" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="A105" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="2">
         <v>45914</v>
       </c>
-      <c r="C105" t="s">
-        <v>10</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="C105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E105" t="s">
-        <v>12</v>
-      </c>
-      <c r="F105" t="s">
+      <c r="E105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="A106" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="2">
         <v>45914</v>
       </c>
-      <c r="C106" t="s">
-        <v>10</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="C106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="2">
         <v>45914</v>
       </c>
-      <c r="C107" t="s">
-        <v>10</v>
-      </c>
-      <c r="D107" t="s">
+      <c r="C107" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="2">
         <v>45910</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F108" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="2">
         <v>46001</v>
       </c>
-      <c r="C109" t="s">
-        <v>10</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E109" t="s">
-        <v>12</v>
-      </c>
-      <c r="F109" t="s">
+      <c r="E109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="2">
         <v>46001</v>
       </c>
-      <c r="C110" t="s">
-        <v>10</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="C110" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111" s="2">
         <v>46001</v>
       </c>
-      <c r="C111" t="s">
-        <v>10</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C111" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112" s="2">
         <v>45946</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F112" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="2">
         <v>45949</v>
       </c>
-      <c r="C113" t="s">
-        <v>10</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="C113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E113" t="s">
-        <v>12</v>
-      </c>
-      <c r="F113" t="s">
+      <c r="E113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="2">
         <v>45949</v>
       </c>
-      <c r="C114" t="s">
-        <v>10</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="C114" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="2">
         <v>45949</v>
       </c>
-      <c r="C115" t="s">
-        <v>10</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="C115" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="2">
         <v>45819</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F116" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117" s="2">
         <v>45972</v>
       </c>
-      <c r="C117" t="s">
-        <v>10</v>
-      </c>
-      <c r="D117" t="s">
+      <c r="C117" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F117" t="s">
+      <c r="F117" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118" s="2">
         <v>45972</v>
       </c>
-      <c r="C118" t="s">
-        <v>10</v>
-      </c>
-      <c r="D118" t="s">
+      <c r="C118" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119" s="2">
         <v>45972</v>
       </c>
-      <c r="C119" t="s">
-        <v>10</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="C119" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B120" s="2">
         <v>45819</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F120" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121" s="2">
         <v>45819</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F121" t="s">
+      <c r="F121" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="2">
         <v>45990</v>
       </c>
-      <c r="C122" t="s">
-        <v>10</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="C122" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F122" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="2">
         <v>45990</v>
       </c>
-      <c r="C123" t="s">
-        <v>10</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="C123" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+      <c r="A124" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="2">
         <v>45759</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F124" t="s">
+      <c r="F124" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B125" s="2">
         <v>45973</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="A126" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126" s="2">
         <v>46004</v>
       </c>
-      <c r="C126" t="s">
-        <v>10</v>
-      </c>
-      <c r="D126" t="s">
+      <c r="C126" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E126" t="s">
-        <v>12</v>
-      </c>
-      <c r="F126" t="s">
+      <c r="E126" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F126" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="A127" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127" s="2">
         <v>46004</v>
       </c>
-      <c r="C127" t="s">
-        <v>10</v>
-      </c>
-      <c r="D127" t="s">
+      <c r="C127" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="A128" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128" s="2">
         <v>45759</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F128" t="s">
+      <c r="F128" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="A129" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129" s="2">
         <v>46010</v>
       </c>
-      <c r="C129" t="s">
-        <v>10</v>
-      </c>
-      <c r="D129" t="s">
+      <c r="C129" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E129" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130" s="2">
         <v>46010</v>
       </c>
-      <c r="C130" t="s">
-        <v>10</v>
-      </c>
-      <c r="D130" t="s">
+      <c r="C130" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="A131" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B131" s="2">
         <v>46039</v>
       </c>
-      <c r="C131" t="s">
-        <v>10</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="C131" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E131" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F131" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="A132" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B132" s="2">
         <v>46047</v>
       </c>
-      <c r="C132" t="s">
-        <v>10</v>
-      </c>
-      <c r="D132" t="s">
+      <c r="C132" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E132">
+      <c r="E132" s="1">
         <v>2</v>
       </c>
-      <c r="F132">
+      <c r="F132" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>400</v>
+      </c>
+      <c r="B133" s="2">
+        <v>46053</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E133" s="1">
+        <v>4</v>
+      </c>
+      <c r="F133" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>400</v>
+      </c>
+      <c r="B134" s="2">
+        <v>46053</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout actions 3ème série IdF
</commit_message>
<xml_diff>
--- a/Data/Actions Simon.xlsx
+++ b/Data/Actions Simon.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zarka/Documents/Simon/Squash/Squash-Data/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7477BAF8-5136-9441-963B-87616C34B712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8750D2-4C4A-3C49-8A49-310C76E80FE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions Simon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -951,7 +951,7 @@
   <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" zoomScale="111" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+      <selection activeCell="I132" sqref="I132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3226,7 +3226,8 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>400</v>
+        <f>400*0.9</f>
+        <v>360</v>
       </c>
       <c r="B134" s="2">
         <v>46053</v>

</xml_diff>